<commit_message>
SECF - exclude securities with huge price fluctations from strategy
</commit_message>
<xml_diff>
--- a/SEC13F/cshares_strategy.xlsx
+++ b/SEC13F/cshares_strategy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24945" windowHeight="9330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24948" windowHeight="9336"/>
   </bookViews>
   <sheets>
     <sheet name="cshares" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cshares!$A$1:$L$116</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId2"/>
+    <pivotCache cacheId="6" r:id="rId2"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -333,7 +333,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -834,7 +834,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -883,64 +883,64 @@
   </cellStyles>
   <dxfs count="21">
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -959,7 +959,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Angela Stanchie" refreshedDate="43081.341639120372" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="115">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Angela Stanchie" refreshedDate="43083.832705555556" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="115">
   <cacheSource type="worksheet">
     <worksheetSource ref="B1:M116" sheet="cshares"/>
   </cacheSource>
@@ -1031,10 +1031,10 @@
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="-227.009871941151" maxValue="27.840015597025996"/>
     </cacheField>
     <cacheField name="gains" numFmtId="44">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-22700.9871941151" maxValue="2784.0015597025995"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-2938.9985556346005" maxValue="2784.0015597025995"/>
     </cacheField>
     <cacheField name="cost" numFmtId="44">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="515.00025071760604" maxValue="26996.997190975202"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="19248.999825675"/>
     </cacheField>
     <cacheField name="Quarters" numFmtId="0" databaseField="0">
       <fieldGroup base="0">
@@ -1449,8 +1449,8 @@
     <n v="210.70993788578301"/>
     <n v="53.34"/>
     <n v="-157.369937885783"/>
-    <n v="-15736.9937885783"/>
-    <n v="21070.9937885783"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="3"/>
@@ -1534,7 +1534,7 @@
     <n v="50.09"/>
     <m/>
     <n v="0"/>
-    <n v="15136.9993632447"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="4"/>
@@ -1575,8 +1575,8 @@
     <n v="236.88012133192299"/>
     <n v="13.53"/>
     <n v="-223.35012133192299"/>
-    <n v="-22335.0121331923"/>
-    <n v="23688.0121331923"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="4"/>
@@ -1589,8 +1589,8 @@
     <n v="86.52"/>
     <n v="13.53"/>
     <n v="-72.989999999999995"/>
-    <n v="-7298.9999999999991"/>
-    <n v="8652"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="4"/>
@@ -1631,8 +1631,8 @@
     <n v="213.37004785001099"/>
     <n v="65.55"/>
     <n v="-147.82004785001101"/>
-    <n v="-14782.004785001101"/>
-    <n v="21337.0047850011"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="4"/>
@@ -1714,9 +1714,9 @@
     <n v="1248141"/>
     <n v="166.62012117316601"/>
     <n v="56.48"/>
-    <m/>
+    <n v="-110.14012117316602"/>
     <n v="0"/>
-    <n v="16662.012117316601"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="5"/>
@@ -1757,8 +1757,8 @@
     <n v="240.87987194115101"/>
     <n v="13.87"/>
     <n v="-227.009871941151"/>
-    <n v="-22700.9871941151"/>
-    <n v="24087.9871941151"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="5"/>
@@ -1771,8 +1771,8 @@
     <n v="86.700010346542797"/>
     <n v="13.87"/>
     <n v="-72.830010346542792"/>
-    <n v="-7283.0010346542795"/>
-    <n v="8670.0010346542804"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="5"/>
@@ -1813,8 +1813,8 @@
     <n v="262.20006456009497"/>
     <n v="65.41"/>
     <n v="-196.79006456009498"/>
-    <n v="-19679.006456009498"/>
-    <n v="26220.006456009498"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="5"/>
@@ -1883,8 +1883,8 @@
     <n v="209.999923823888"/>
     <n v="13.53"/>
     <n v="-196.469923823888"/>
-    <n v="-19646.992382388798"/>
-    <n v="20999.992382388798"/>
+    <n v="0"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="6"/>
@@ -1952,9 +1952,9 @@
     <n v="2535542"/>
     <n v="171.250046096869"/>
     <n v="51.44"/>
-    <m/>
+    <n v="-119.810046096869"/>
     <n v="0"/>
-    <n v="17125.004609686901"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="7"/>
@@ -2038,7 +2038,7 @@
     <n v="51.65"/>
     <m/>
     <n v="0"/>
-    <n v="17585.001093701099"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="8"/>
@@ -2192,7 +2192,7 @@
     <n v="59.4"/>
     <m/>
     <n v="0"/>
-    <n v="20243.0026020638"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="10"/>
@@ -2346,7 +2346,7 @@
     <n v="285.77"/>
     <m/>
     <n v="0"/>
-    <n v="26996.997190975202"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="12"/>
@@ -2688,7 +2688,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="O1:Q23" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
@@ -3329,24 +3329,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5546875" customWidth="1"/>
+    <col min="16" max="16" width="10.88671875" customWidth="1"/>
+    <col min="17" max="17" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3393,7 +3394,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>340</v>
       </c>
@@ -3442,7 +3443,7 @@
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>631</v>
       </c>
@@ -3495,7 +3496,7 @@
         <v>2319.9974643993792</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>533</v>
       </c>
@@ -3548,7 +3549,7 @@
         <v>869.99350019630083</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>344</v>
       </c>
@@ -3597,7 +3598,7 @@
       <c r="P5" s="10"/>
       <c r="Q5" s="10"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>684</v>
       </c>
@@ -3650,7 +3651,7 @@
         <v>-2013.0041036756004</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>107</v>
       </c>
@@ -3697,13 +3698,13 @@
         <v>93</v>
       </c>
       <c r="P7" s="10">
-        <v>82959.008668349619</v>
+        <v>61888.014879771319</v>
       </c>
       <c r="Q7" s="10">
-        <v>-17451.008668349608</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+        <v>-1714.0148797713096</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3750,13 +3751,13 @@
         <v>89</v>
       </c>
       <c r="P8" s="10">
-        <v>126830.01451375654</v>
+        <v>58015.998232318438</v>
       </c>
       <c r="Q8" s="10">
-        <v>-45435.015150511841</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+        <v>-1018.998232318432</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>512</v>
       </c>
@@ -3803,13 +3804,13 @@
         <v>90</v>
       </c>
       <c r="P9" s="10">
-        <v>134258.5187056672</v>
+        <v>58618.511903571722</v>
       </c>
       <c r="Q9" s="10">
-        <v>-49856.506588350596</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+        <v>-193.51190357171851</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>61</v>
       </c>
@@ -3858,7 +3859,7 @@
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>86</v>
       </c>
@@ -3905,13 +3906,13 @@
         <v>92</v>
       </c>
       <c r="P11" s="10">
-        <v>73410.997663547751</v>
+        <v>52411.005281158948</v>
       </c>
       <c r="Q11" s="10">
-        <v>-18096.997663547751</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1549.9947188410497</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>611</v>
       </c>
@@ -3958,13 +3959,13 @@
         <v>93</v>
       </c>
       <c r="P12" s="10">
-        <v>21465.005258851539</v>
+        <v>4340.00064916464</v>
       </c>
       <c r="Q12" s="10">
         <v>-239.00064916464032</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>377</v>
       </c>
@@ -4011,13 +4012,13 @@
         <v>89</v>
       </c>
       <c r="P13" s="10">
-        <v>50728.007441044967</v>
+        <v>33143.006347343871</v>
       </c>
       <c r="Q13" s="10">
         <v>-2901.0063473438699</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>511</v>
       </c>
@@ -4070,7 +4071,7 @@
         <v>-1151.010487776141</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>658</v>
       </c>
@@ -4119,7 +4120,7 @@
       <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>20</v>
       </c>
@@ -4166,13 +4167,13 @@
         <v>92</v>
       </c>
       <c r="P16" s="10">
-        <v>70736.006129209462</v>
+        <v>50493.003527145651</v>
       </c>
       <c r="Q16" s="10">
         <v>-3502.00352714566</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>133</v>
       </c>
@@ -4225,7 +4226,7 @@
         <v>1466.9954862887382</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>103</v>
       </c>
@@ -4272,13 +4273,13 @@
         <v>89</v>
       </c>
       <c r="P18" s="10">
-        <v>68820.021271064252</v>
+        <v>41823.024080089053</v>
       </c>
       <c r="Q18" s="10">
         <v>345.97591991094987</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>403</v>
       </c>
@@ -4331,7 +4332,7 @@
         <v>1782.999701529538</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>357</v>
       </c>
@@ -4380,7 +4381,7 @@
       <c r="P20" s="10"/>
       <c r="Q20" s="10"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>252</v>
       </c>
@@ -4433,7 +4434,7 @@
         <v>2684.9913175294346</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>113</v>
       </c>
@@ -4486,7 +4487,7 @@
         <v>-1666.999999759541</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>271</v>
       </c>
@@ -4533,13 +4534,13 @@
         <v>87</v>
       </c>
       <c r="P23" s="10">
-        <v>898993.61677275947</v>
+        <v>630518.60202183155</v>
       </c>
       <c r="Q23" s="10">
-        <v>-132841.59979577092</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+        <v>-3378.6020218315234</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>552</v>
       </c>
@@ -4583,7 +4584,7 @@
         <v>4422.0034042308198</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>296</v>
       </c>
@@ -4627,7 +4628,7 @@
         <v>4263.0023823802294</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>493</v>
       </c>
@@ -4671,7 +4672,7 @@
         <v>4331.9979898244401</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>13</v>
       </c>
@@ -4715,51 +4716,49 @@
         <v>3013.0006612991501</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
         <v>519</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="5">
         <v>41820</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="4">
         <v>379225000</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="4">
         <v>43464000</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="4">
         <v>1799749</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="4">
         <v>244290</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="4">
         <v>210.70993788578301</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="4">
         <v>53.34</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="4">
         <f t="shared" si="0"/>
         <v>-157.369937885783</v>
       </c>
-      <c r="L28" s="6">
-        <f t="shared" si="1"/>
-        <v>-15736.9937885783</v>
-      </c>
-      <c r="M28" s="6">
-        <f t="shared" si="2"/>
-        <v>21070.9937885783</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L28" s="7">
+        <v>0</v>
+      </c>
+      <c r="M28" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>156</v>
       </c>
@@ -4803,7 +4802,7 @@
         <v>4881.0011551790503</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>603</v>
       </c>
@@ -4847,7 +4846,7 @@
         <v>4893.0039528221205</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>577</v>
       </c>
@@ -4891,7 +4890,7 @@
         <v>7506.9996035019303</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>333</v>
       </c>
@@ -4935,7 +4934,7 @@
         <v>3194</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>30</v>
       </c>
@@ -4979,7 +4978,7 @@
         <v>18982.9985556346</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>467</v>
       </c>
@@ -5015,12 +5014,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M34" s="6">
-        <f t="shared" si="2"/>
-        <v>15136.9993632447</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M34" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>688</v>
       </c>
@@ -5064,7 +5062,7 @@
         <v>4254.00155965668</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>573</v>
       </c>
@@ -5108,95 +5106,91 @@
         <v>7391.9921957840306</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="4">
         <v>210</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="5">
         <v>41912</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="4">
         <v>493237000</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="4">
         <v>19578000</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="4">
         <v>2082222</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="4">
         <v>205600</v>
       </c>
-      <c r="I37">
+      <c r="I37" s="4">
         <v>236.88012133192299</v>
       </c>
-      <c r="J37">
+      <c r="J37" s="4">
         <v>13.53</v>
       </c>
-      <c r="K37">
+      <c r="K37" s="4">
         <f t="shared" si="0"/>
         <v>-223.35012133192299</v>
       </c>
-      <c r="L37" s="6">
-        <f t="shared" si="1"/>
-        <v>-22335.0121331923</v>
-      </c>
-      <c r="M37" s="6">
-        <f t="shared" si="2"/>
-        <v>23688.0121331923</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="L37" s="7">
+        <v>0</v>
+      </c>
+      <c r="M37" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="4">
         <v>388</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="5">
         <v>41912</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="4">
         <v>2595600000</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="4">
         <v>600586000</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="4">
         <v>30000000</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="4">
         <v>6532005</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="4">
         <v>86.52</v>
       </c>
-      <c r="J38">
+      <c r="J38" s="4">
         <v>13.53</v>
       </c>
-      <c r="K38">
+      <c r="K38" s="4">
         <f t="shared" si="0"/>
         <v>-72.989999999999995</v>
       </c>
-      <c r="L38" s="6">
-        <f t="shared" si="1"/>
-        <v>-7298.9999999999991</v>
-      </c>
-      <c r="M38" s="6">
-        <f t="shared" si="2"/>
-        <v>8652</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L38" s="7">
+        <v>0</v>
+      </c>
+      <c r="M38" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>163</v>
       </c>
@@ -5240,7 +5234,7 @@
         <v>3615.0003274211699</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>619</v>
       </c>
@@ -5284,51 +5278,49 @@
         <v>5237.0049893550704</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="4">
         <v>665</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="5">
         <v>41912</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="4">
         <v>457954000</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="4">
         <v>78729000</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="4">
         <v>2146290</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="4">
         <v>346541</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="4">
         <v>213.37004785001099</v>
       </c>
-      <c r="J41">
+      <c r="J41" s="4">
         <v>65.55</v>
       </c>
-      <c r="K41">
+      <c r="K41" s="4">
         <f t="shared" si="0"/>
         <v>-147.82004785001101</v>
       </c>
-      <c r="L41" s="6">
-        <f t="shared" si="1"/>
-        <v>-14782.004785001101</v>
-      </c>
-      <c r="M41" s="6">
-        <f t="shared" si="2"/>
-        <v>21337.0047850011</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L41" s="7">
+        <v>0</v>
+      </c>
+      <c r="M41" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>49</v>
       </c>
@@ -5372,7 +5364,7 @@
         <v>7694.0011935341599</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>439</v>
       </c>
@@ -5416,7 +5408,7 @@
         <v>7646.9994109327199</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>26</v>
       </c>
@@ -5460,7 +5452,7 @@
         <v>7573.9992952262892</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>117</v>
       </c>
@@ -5504,7 +5496,7 @@
         <v>3491.0024390243898</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>269</v>
       </c>
@@ -5548,7 +5540,7 @@
         <v>16043.999584938998</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>599</v>
       </c>
@@ -5579,17 +5571,18 @@
       <c r="J47" s="4">
         <v>56.48</v>
       </c>
-      <c r="K47" s="4"/>
+      <c r="K47" s="7">
+        <f t="shared" si="0"/>
+        <v>-110.14012117316602</v>
+      </c>
       <c r="L47" s="7">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M47" s="6">
-        <f t="shared" si="2"/>
-        <v>16662.012117316601</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M47" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>549</v>
       </c>
@@ -5633,7 +5626,7 @@
         <v>5020.5041934764504</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>432</v>
       </c>
@@ -5677,95 +5670,91 @@
         <v>8616.0004266859505</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" s="4">
         <v>75</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50" s="5">
         <v>42004</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="4">
         <v>687396000</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="4">
         <v>194159000</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="4">
         <v>2853688</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="4">
         <v>771466</v>
       </c>
-      <c r="I50">
+      <c r="I50" s="4">
         <v>240.87987194115101</v>
       </c>
-      <c r="J50">
+      <c r="J50" s="4">
         <v>13.87</v>
       </c>
-      <c r="K50">
+      <c r="K50" s="4">
         <f t="shared" si="0"/>
         <v>-227.009871941151</v>
       </c>
-      <c r="L50" s="6">
-        <f t="shared" si="1"/>
-        <v>-22700.9871941151</v>
-      </c>
-      <c r="M50" s="6">
-        <f t="shared" si="2"/>
-        <v>24087.9871941151</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="L50" s="7">
+        <v>0</v>
+      </c>
+      <c r="M50" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" s="4">
         <v>624</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="5">
         <v>42004</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="4">
         <v>2718346000</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="4">
         <v>122746000</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="4">
         <v>31353468</v>
       </c>
-      <c r="H51">
+      <c r="H51" s="4">
         <v>1353468</v>
       </c>
-      <c r="I51">
+      <c r="I51" s="4">
         <v>86.700010346542797</v>
       </c>
-      <c r="J51">
+      <c r="J51" s="4">
         <v>13.87</v>
       </c>
-      <c r="K51">
+      <c r="K51" s="4">
         <f t="shared" si="0"/>
         <v>-72.830010346542792</v>
       </c>
-      <c r="L51" s="6">
-        <f t="shared" si="1"/>
-        <v>-7283.0010346542795</v>
-      </c>
-      <c r="M51" s="6">
-        <f t="shared" si="2"/>
-        <v>8670.0010346542804</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L51" s="7">
+        <v>0</v>
+      </c>
+      <c r="M51" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>472</v>
       </c>
@@ -5809,7 +5798,7 @@
         <v>7170.0012181009797</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>298</v>
       </c>
@@ -5853,51 +5842,49 @@
         <v>3178.0024007915399</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A54" s="4">
         <v>518</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54" s="5">
         <v>42004</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="4">
         <v>657936000</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="4">
         <v>199982000</v>
       </c>
-      <c r="G54">
+      <c r="G54" s="4">
         <v>2509290</v>
       </c>
-      <c r="H54">
+      <c r="H54" s="4">
         <v>363000</v>
       </c>
-      <c r="I54">
+      <c r="I54" s="4">
         <v>262.20006456009497</v>
       </c>
-      <c r="J54">
+      <c r="J54" s="4">
         <v>65.41</v>
       </c>
-      <c r="K54">
+      <c r="K54" s="4">
         <f t="shared" si="0"/>
         <v>-196.79006456009498</v>
       </c>
-      <c r="L54" s="6">
-        <f t="shared" si="1"/>
-        <v>-19679.006456009498</v>
-      </c>
-      <c r="M54" s="6">
-        <f t="shared" si="2"/>
-        <v>26220.006456009498</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L54" s="7">
+        <v>0</v>
+      </c>
+      <c r="M54" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>275</v>
       </c>
@@ -5941,7 +5928,7 @@
         <v>7525.0023453271197</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>508</v>
       </c>
@@ -5985,7 +5972,7 @@
         <v>8769.0012010336213</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>330</v>
       </c>
@@ -6029,7 +6016,7 @@
         <v>3384.0031714342304</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>21</v>
       </c>
@@ -6073,51 +6060,49 @@
         <v>16050.000053415401</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A59" s="4">
         <v>223</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="5">
         <v>42094</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E59">
+      <c r="E59" s="4">
         <v>882166000</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="4">
         <v>194770000</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="4">
         <v>4200792</v>
       </c>
-      <c r="H59">
+      <c r="H59" s="4">
         <v>1347104</v>
       </c>
-      <c r="I59">
+      <c r="I59" s="4">
         <v>209.999923823888</v>
       </c>
-      <c r="J59">
+      <c r="J59" s="4">
         <v>13.53</v>
       </c>
-      <c r="K59">
+      <c r="K59" s="4">
         <f t="shared" si="0"/>
         <v>-196.469923823888</v>
       </c>
-      <c r="L59" s="6">
-        <f t="shared" si="1"/>
-        <v>-19646.992382388798</v>
-      </c>
-      <c r="M59" s="6">
-        <f t="shared" si="2"/>
-        <v>20999.992382388798</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L59" s="7">
+        <v>0</v>
+      </c>
+      <c r="M59" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>722</v>
       </c>
@@ -6161,7 +6146,7 @@
         <v>7860.0030668915697</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>717</v>
       </c>
@@ -6205,7 +6190,7 @@
         <v>4367.0012637664495</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>674</v>
       </c>
@@ -6249,7 +6234,7 @@
         <v>6540.9968073354403</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>247</v>
       </c>
@@ -6293,7 +6278,7 @@
         <v>5439.9997172822405</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
         <v>407</v>
       </c>
@@ -6324,17 +6309,18 @@
       <c r="J64" s="4">
         <v>51.44</v>
       </c>
-      <c r="K64" s="4"/>
+      <c r="K64" s="4">
+        <f t="shared" si="0"/>
+        <v>-119.810046096869</v>
+      </c>
       <c r="L64" s="7">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M64" s="6">
-        <f t="shared" si="2"/>
-        <v>17125.004609686901</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M64" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>669</v>
       </c>
@@ -6378,7 +6364,7 @@
         <v>4340.00064916464</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>301</v>
       </c>
@@ -6422,7 +6408,7 @@
         <v>2534.0014174459297</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>166</v>
       </c>
@@ -6466,7 +6452,7 @@
         <v>2698.0064163137299</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>171</v>
       </c>
@@ -6510,7 +6496,7 @@
         <v>3002</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>191</v>
       </c>
@@ -6554,7 +6540,7 @@
         <v>14496.999695804601</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="4">
         <v>627</v>
       </c>
@@ -6590,12 +6576,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M70" s="6">
-        <f t="shared" si="5"/>
-        <v>17585.001093701099</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M70" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>487</v>
       </c>
@@ -6639,7 +6624,7 @@
         <v>4294.0015229209603</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>160</v>
       </c>
@@ -6683,7 +6668,7 @@
         <v>3445.9972948586496</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>353</v>
       </c>
@@ -6727,7 +6712,7 @@
         <v>2672</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>732</v>
       </c>
@@ -6771,7 +6756,7 @@
         <v>2665.0017149717</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>358</v>
       </c>
@@ -6815,7 +6800,7 @@
         <v>7627.00384327143</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>154</v>
       </c>
@@ -6859,7 +6844,7 @@
         <v>4236.0049539647298</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>380</v>
       </c>
@@ -6903,7 +6888,7 @@
         <v>5435.9999755682802</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>327</v>
       </c>
@@ -6947,7 +6932,7 @@
         <v>3682.9989534845099</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>125</v>
       </c>
@@ -6991,7 +6976,7 @@
         <v>7699.0011680772695</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>381</v>
       </c>
@@ -7035,7 +7020,7 @@
         <v>15144.998412762001</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="4">
         <v>73</v>
       </c>
@@ -7071,12 +7056,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M81" s="6">
-        <f t="shared" si="5"/>
-        <v>20243.0026020638</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M81" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>300</v>
       </c>
@@ -7120,7 +7104,7 @@
         <v>3850.0045835527799</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>709</v>
       </c>
@@ -7164,7 +7148,7 @@
         <v>3809.0000000000005</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>347</v>
       </c>
@@ -7208,7 +7192,7 @@
         <v>8658.9999873594898</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>310</v>
       </c>
@@ -7252,7 +7236,7 @@
         <v>7648.0004219096099</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>424</v>
       </c>
@@ -7296,7 +7280,7 @@
         <v>9559.997956356121</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>189</v>
       </c>
@@ -7340,7 +7324,7 @@
         <v>2905.9998615162799</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>161</v>
       </c>
@@ -7384,7 +7368,7 @@
         <v>3225.9929999919004</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>22</v>
       </c>
@@ -7428,7 +7412,7 @@
         <v>3249.0148128533797</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>276</v>
       </c>
@@ -7472,7 +7456,7 @@
         <v>7933.998882993581</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>12</v>
       </c>
@@ -7516,7 +7500,7 @@
         <v>3987.9996472488201</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" s="4">
         <v>101</v>
       </c>
@@ -7552,12 +7536,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M92" s="6">
-        <f t="shared" si="5"/>
-        <v>26996.997190975202</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M92" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>66</v>
       </c>
@@ -7601,7 +7584,7 @@
         <v>3417.9997053649304</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>63</v>
       </c>
@@ -7645,7 +7628,7 @@
         <v>3398.0097029466697</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>679</v>
       </c>
@@ -7689,7 +7672,7 @@
         <v>3341.0026907135602</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>35</v>
       </c>
@@ -7733,7 +7716,7 @@
         <v>8055.00024711893</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>104</v>
       </c>
@@ -7777,7 +7760,7 @@
         <v>8270.0052828602402</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>236</v>
       </c>
@@ -7821,7 +7804,7 @@
         <v>11353.0068038359</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>566</v>
       </c>
@@ -7865,7 +7848,7 @@
         <v>4668.99948784554</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>616</v>
       </c>
@@ -7909,7 +7892,7 @@
         <v>11581.998440297401</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>77</v>
       </c>
@@ -7953,7 +7936,7 @@
         <v>4738.0005019386999</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>363</v>
       </c>
@@ -7997,7 +7980,7 @@
         <v>4919.0005096958403</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>421</v>
       </c>
@@ -8041,7 +8024,7 @@
         <v>7288.0013586929808</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>349</v>
       </c>
@@ -8085,7 +8068,7 @@
         <v>4230.0009655256999</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>320</v>
       </c>
@@ -8129,7 +8112,7 @@
         <v>14365.999344481301</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>501</v>
       </c>
@@ -8173,7 +8156,7 @@
         <v>4723.0013735283801</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>548</v>
       </c>
@@ -8217,7 +8200,7 @@
         <v>3892.0060891118096</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>200</v>
       </c>
@@ -8261,7 +8244,7 @@
         <v>3878.0014030504803</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>211</v>
       </c>
@@ -8305,7 +8288,7 @@
         <v>5375.9992560552901</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>428</v>
       </c>
@@ -8349,7 +8332,7 @@
         <v>515.00025071760604</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>746</v>
       </c>
@@ -8393,7 +8376,7 @@
         <v>17250</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>739</v>
       </c>
@@ -8437,7 +8420,7 @@
         <v>5132.9999999203601</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>738</v>
       </c>
@@ -8481,7 +8464,7 @@
         <v>4234</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>747</v>
       </c>
@@ -8525,7 +8508,7 @@
         <v>4085</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>735</v>
       </c>
@@ -8569,7 +8552,7 @@
         <v>4092.99999983918</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>736</v>
       </c>

</xml_diff>

<commit_message>
SEC13F -> bold grand total
</commit_message>
<xml_diff>
--- a/SEC13F/cshares_strategy.xlsx
+++ b/SEC13F/cshares_strategy.xlsx
@@ -19,7 +19,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -2688,7 +2688,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="O1:Q23" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
@@ -3327,10 +3327,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q116"/>
+  <dimension ref="A1:R116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3347,7 +3347,7 @@
     <col min="17" max="17" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>340</v>
       </c>
@@ -3443,7 +3443,7 @@
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>631</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>2319.9974643993792</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>533</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>869.99350019630083</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>344</v>
       </c>
@@ -3597,8 +3597,12 @@
       </c>
       <c r="P5" s="10"/>
       <c r="Q5" s="10"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R5" s="10">
+        <f>SUM(Q3:Q5)</f>
+        <v>3189.99096459568</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>684</v>
       </c>
@@ -3651,7 +3655,7 @@
         <v>-2013.0041036756004</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>107</v>
       </c>
@@ -3704,7 +3708,7 @@
         <v>-1714.0148797713096</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3757,7 +3761,7 @@
         <v>-1018.998232318432</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>512</v>
       </c>
@@ -3810,7 +3814,7 @@
         <v>-193.51190357171851</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>61</v>
       </c>
@@ -3858,8 +3862,12 @@
       </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R10" s="10">
+        <f>SUM(Q6:Q10)</f>
+        <v>-4939.5291193370613</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>86</v>
       </c>
@@ -3912,7 +3920,7 @@
         <v>1549.9947188410497</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>611</v>
       </c>
@@ -3965,7 +3973,7 @@
         <v>-239.00064916464032</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>377</v>
       </c>
@@ -4018,7 +4026,7 @@
         <v>-2901.0063473438699</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>511</v>
       </c>
@@ -4071,7 +4079,7 @@
         <v>-1151.010487776141</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>658</v>
       </c>
@@ -4119,8 +4127,12 @@
       </c>
       <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R15" s="10">
+        <f>SUM(Q11:Q15)</f>
+        <v>-2741.0227654436017</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>20</v>
       </c>
@@ -4173,7 +4185,7 @@
         <v>-3502.00352714566</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>133</v>
       </c>
@@ -4226,7 +4238,7 @@
         <v>1466.9954862887382</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>103</v>
       </c>
@@ -4279,7 +4291,7 @@
         <v>345.97591991094987</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>403</v>
       </c>
@@ -4332,7 +4344,7 @@
         <v>1782.999701529538</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>357</v>
       </c>
@@ -4380,8 +4392,12 @@
       </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="10"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R20" s="10">
+        <f>SUM(Q16:Q20)</f>
+        <v>93.967580583566132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>252</v>
       </c>
@@ -4434,7 +4450,7 @@
         <v>2684.9913175294346</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>113</v>
       </c>
@@ -4486,8 +4502,12 @@
       <c r="Q22" s="10">
         <v>-1666.999999759541</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R22" s="10">
+        <f>SUM(Q21:Q22)</f>
+        <v>1017.9913177698936</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>271</v>
       </c>
@@ -4539,8 +4559,12 @@
       <c r="Q23" s="10">
         <v>-3378.6020218315234</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R23">
+        <f>SUM(R3:R22)</f>
+        <v>-3378.6020218315234</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>552</v>
       </c>
@@ -4584,7 +4608,7 @@
         <v>4422.0034042308198</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>296</v>
       </c>
@@ -4628,7 +4652,7 @@
         <v>4263.0023823802294</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>493</v>
       </c>
@@ -4672,7 +4696,7 @@
         <v>4331.9979898244401</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>13</v>
       </c>
@@ -4716,7 +4740,7 @@
         <v>3013.0006612991501</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>519</v>
       </c>
@@ -4758,7 +4782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>156</v>
       </c>
@@ -4802,7 +4826,7 @@
         <v>4881.0011551790503</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>603</v>
       </c>
@@ -4846,7 +4870,7 @@
         <v>4893.0039528221205</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>577</v>
       </c>
@@ -4890,7 +4914,7 @@
         <v>7506.9996035019303</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>333</v>
       </c>

</xml_diff>